<commit_message>
Pushing a pic for testing
</commit_message>
<xml_diff>
--- a/raw_dataset/Crime_data_A_original.xlsx
+++ b/raw_dataset/Crime_data_A_original.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihle\Python_programs\Capestone_simulation\raw_dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b723dd9e2080892/Zaio Projects/Capestone_simulation/raw_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70185098-092D-4F13-AAE2-DFFA9256BBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{70185098-092D-4F13-AAE2-DFFA9256BBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{273C6AB9-8922-40C2-AD90-F1CF70ECD5E3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{55222D71-3E38-40FA-919F-BB69B2DA5D0B}"/>
   </bookViews>
@@ -1654,10 +1654,25 @@
   <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
@@ -3747,13 +3762,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D6:D13 D15:D18 D20:D26">
-    <cfRule type="cellIs" dxfId="58" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="34" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="59" priority="33" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="34" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="32" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3769,13 +3784,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47:D51">
+    <cfRule type="cellIs" dxfId="54" priority="28" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="53" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="52" priority="27" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="28" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3794,53 +3809,53 @@
     <cfRule type="containsText" dxfId="48" priority="22" operator="containsText" text="0 count diff">
       <formula>NOT(ISERROR(SEARCH("0 count diff",E6)))</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="24" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="46" priority="23" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="24" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
     <cfRule type="cellIs" dxfId="45" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:E30 E32:E37 E39:E42 E44">
+    <cfRule type="cellIs" dxfId="44" priority="18" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="19" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="15" operator="containsText" text="high">
+      <formula>NOT(ISERROR(SEARCH("high",E28)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="41" priority="14" operator="containsText" text="low">
       <formula>NOT(ISERROR(SEARCH("low",E28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="15" operator="containsText" text="high">
-      <formula>NOT(ISERROR(SEARCH("high",E28)))</formula>
-    </cfRule>
     <cfRule type="containsText" dxfId="40" priority="16" operator="containsText" text="0 count diff">
       <formula>NOT(ISERROR(SEARCH("0 count diff",E28)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="39" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="18" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="19" operator="equal">
-      <formula>0</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47:E51">
+    <cfRule type="containsText" dxfId="38" priority="9" operator="containsText" text="high">
+      <formula>NOT(ISERROR(SEARCH("high",E47)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="10" operator="containsText" text="0 count diff">
+      <formula>NOT(ISERROR(SEARCH("0 count diff",E47)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="11" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="35" priority="8" operator="containsText" text="low">
       <formula>NOT(ISERROR(SEARCH("low",E47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="9" operator="containsText" text="high">
-      <formula>NOT(ISERROR(SEARCH("high",E47)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="10" operator="containsText" text="0 count diff">
-      <formula>NOT(ISERROR(SEARCH("0 count diff",E47)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="33" priority="12" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3865,14 +3880,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:O13">
+    <cfRule type="expression" dxfId="26" priority="61">
+      <formula>Y6=0</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="25" priority="59">
       <formula>Y6&lt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="24" priority="60">
       <formula>Y6&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="61">
-      <formula>Y6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15:O18">
@@ -3887,80 +3902,80 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:O26">
+    <cfRule type="expression" dxfId="20" priority="55">
+      <formula>Y20=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="54">
+      <formula>Y20&gt;0</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="18" priority="53">
       <formula>Y20&lt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="54">
-      <formula>Y20&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="55">
-      <formula>Y20=0</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28:O30">
+    <cfRule type="expression" dxfId="17" priority="52">
+      <formula>Y28=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="51">
+      <formula>Y28&gt;0</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="15" priority="50">
       <formula>Y28&lt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="51">
-      <formula>Y28&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="52">
-      <formula>Y28=0</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:O37">
+    <cfRule type="expression" dxfId="14" priority="49">
+      <formula>Y32=0</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="13" priority="47">
       <formula>Y32&lt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="12" priority="48">
       <formula>Y32&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="49">
-      <formula>Y32=0</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39:O42">
+    <cfRule type="expression" dxfId="11" priority="45">
+      <formula>Y39&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="46">
+      <formula>Y39=0</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="9" priority="44">
       <formula>Y39&lt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="45">
-      <formula>Y39&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="46">
-      <formula>Y39=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G44:O44">
     <cfRule type="expression" dxfId="8" priority="41">
       <formula>Y44&lt;0</formula>
     </cfRule>
+    <cfRule type="expression" dxfId="7" priority="43">
+      <formula>Y44=0</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="6" priority="42">
       <formula>Y44&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="43">
-      <formula>Y44=0</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47:O51">
+    <cfRule type="expression" dxfId="5" priority="40">
+      <formula>Y47=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="39">
+      <formula>Y47&lt;0</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="3" priority="38">
       <formula>Y47&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="39">
-      <formula>Y47&lt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="40">
-      <formula>Y47=0</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G55:O55">
+    <cfRule type="expression" dxfId="2" priority="37">
+      <formula>Y55=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="36">
+      <formula>Y55&gt;0</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="0" priority="35">
       <formula>Y55&lt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="36">
-      <formula>Y55&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="37">
-      <formula>Y55=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Limpopo and Western Cape vs National statistics Bar Graph completed.
</commit_message>
<xml_diff>
--- a/raw_dataset/Crime_data_A_original.xlsx
+++ b/raw_dataset/Crime_data_A_original.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6b723dd9e2080892/Zaio Projects/Capestone_simulation/raw_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{70185098-092D-4F13-AAE2-DFFA9256BBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{273C6AB9-8922-40C2-AD90-F1CF70ECD5E3}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{70185098-092D-4F13-AAE2-DFFA9256BBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B06C27E2-3D72-4632-A39F-0E8CC5EBDAE3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{55222D71-3E38-40FA-919F-BB69B2DA5D0B}"/>
   </bookViews>
@@ -683,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
@@ -958,6 +958,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1651,10 +1652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1585A7DD-C699-4C4E-BD2E-7C8E0F207DA6}">
-  <dimension ref="A1:O56"/>
+  <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1674,7 +1675,7 @@
     <col min="15" max="15" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1691,7 +1692,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1708,7 +1709,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1725,7 +1726,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="58.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1770,7 +1771,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
@@ -1789,7 +1790,7 @@
       <c r="N5" s="11"/>
       <c r="O5" s="14"/>
     </row>
-    <row r="6" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>15</v>
       </c>
@@ -1833,8 +1834,9 @@
       <c r="O6" s="22">
         <v>1063</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P6" s="70"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>16</v>
       </c>
@@ -1879,7 +1881,7 @@
         <v>1546</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>17</v>
       </c>
@@ -1924,7 +1926,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>18</v>
       </c>
@@ -1969,7 +1971,7 @@
         <v>5350</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>19</v>
       </c>
@@ -2014,7 +2016,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>20</v>
       </c>
@@ -2059,7 +2061,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="30" t="s">
         <v>21</v>
       </c>
@@ -2104,7 +2106,7 @@
         <v>6227</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="37" t="s">
         <v>22</v>
       </c>
@@ -2149,7 +2151,7 @@
         <v>27924</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="44" t="s">
         <v>23</v>
       </c>
@@ -2168,7 +2170,7 @@
       <c r="N14" s="45"/>
       <c r="O14" s="48"/>
     </row>
-    <row r="15" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>24</v>
       </c>
@@ -2213,7 +2215,7 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="23" t="s">
         <v>25</v>
       </c>
@@ -3979,5 +3981,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>